<commit_message>
turn in main project file
</commit_message>
<xml_diff>
--- a/clustering/models.xlsx
+++ b/clustering/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddfloww/Documents/_datasci/ds-methodologies-exercises/clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1985D251-DAD8-C949-BD98-244E3164B833}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8858EB16-69D9-1A4E-B69A-36621CDAD2EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{ABD91C3E-A360-2848-8706-7CB331435585}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>'calculatedfinishedsquarefeet'</t>
   </si>
@@ -51,12 +51,6 @@
     <t>'calculatedfinishedsquarefeet', 'taxamount', 'latitude', 'longitude', 'lotsizesquarefeet'</t>
   </si>
   <si>
-    <t>'cluster_target_a', 'cluster_target_b', 'cluster_target_c'</t>
-  </si>
-  <si>
-    <t>'cluster_target_a', 'cluster_target_b'</t>
-  </si>
-  <si>
     <t>'cluster_target_c'</t>
   </si>
   <si>
@@ -79,13 +73,25 @@
   </si>
   <si>
     <t>lm7</t>
+  </si>
+  <si>
+    <t>lm8</t>
+  </si>
+  <si>
+    <t>'cluster_target_b', 'cluster_target_c'</t>
+  </si>
+  <si>
+    <t>'cluster_target_b'</t>
+  </si>
+  <si>
+    <t>all numerical variables besides logerror</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +110,15 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -151,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -174,12 +189,6 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -191,6 +200,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BF9150-9879-D246-BB5C-274753BF3C63}">
-  <dimension ref="E6:H13"/>
+  <dimension ref="E6:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -522,7 +543,7 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:8" ht="25">
-      <c r="E6" s="11"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
         <v>1</v>
@@ -532,8 +553,8 @@
       </c>
     </row>
     <row r="7" spans="5:8" ht="63" customHeight="1">
-      <c r="E7" s="13" t="s">
-        <v>9</v>
+      <c r="E7" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>0</v>
@@ -546,8 +567,8 @@
       </c>
     </row>
     <row r="8" spans="5:8" ht="63" customHeight="1">
-      <c r="E8" s="13" t="s">
-        <v>10</v>
+      <c r="E8" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>3</v>
@@ -561,26 +582,26 @@
     </row>
     <row r="9" spans="5:8" ht="63" customHeight="1">
       <c r="E9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="14">
         <v>2.3E-2</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="15">
         <v>2.98E-2</v>
       </c>
     </row>
     <row r="10" spans="5:8" ht="63" customHeight="1">
-      <c r="E10" s="13" t="s">
-        <v>12</v>
+      <c r="E10" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="8">
         <v>2.3599999999999999E-2</v>
       </c>
       <c r="H10" s="7">
@@ -588,45 +609,59 @@
       </c>
     </row>
     <row r="11" spans="5:8" ht="63" customHeight="1">
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="8">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="H11" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" ht="63" customHeight="1">
+      <c r="E12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="8">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" ht="63" customHeight="1">
+      <c r="E13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="G11" s="8">
-        <v>4.8700000000000002E-3</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0.7944</v>
-      </c>
-    </row>
-    <row r="12" spans="5:8" ht="63" customHeight="1">
-      <c r="E12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="10">
-        <v>4.8700000000000002E-3</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0.7944</v>
-      </c>
-    </row>
-    <row r="13" spans="5:8" ht="63" customHeight="1">
-      <c r="E13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>8</v>
       </c>
       <c r="G13" s="6">
         <v>2.3699999999999999E-2</v>
       </c>
       <c r="H13" s="7">
         <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" ht="22">
+      <c r="E14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="14">
+        <v>2.29E-2</v>
+      </c>
+      <c r="H14" s="15">
+        <v>3.1399999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>